<commit_message>
Important : Stable version , Like + Message Only , no UI
</commit_message>
<xml_diff>
--- a/Selenium_Project/instagram_SmallData.xlsx
+++ b/Selenium_Project/instagram_SmallData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\Web_Automation\Selenium_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0EFD11-58C3-420D-BAA9-B271EF675420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25C17F3-DBBA-475E-B21E-327DA3E3175D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7785" xr2:uid="{1BAA3D43-5EC4-499E-ADF4-0A10EC7C61AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1BAA3D43-5EC4-499E-ADF4-0A10EC7C61AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,366 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>pawsandmoorecrochet</t>
-  </si>
-  <si>
-    <t>rupert_the_pom_bear</t>
-  </si>
-  <si>
-    <t>mikkomorkie</t>
-  </si>
-  <si>
-    <t>sharonjiva</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="120">
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>paco.taco.dorado</t>
+  </si>
+  <si>
+    <t>marion_catsanddogs</t>
+  </si>
+  <si>
+    <t>phillyfosterlove</t>
+  </si>
+  <si>
+    <t>keeping_up_with_phoenix</t>
+  </si>
+  <si>
+    <t>simuk_e</t>
+  </si>
+  <si>
+    <t>thebengalsimba2024</t>
+  </si>
+  <si>
+    <t>eddiepateddie</t>
+  </si>
+  <si>
+    <t>bambi_and_thistle</t>
+  </si>
+  <si>
+    <t>leos.whinery</t>
+  </si>
+  <si>
+    <t>aleahrdun</t>
+  </si>
+  <si>
+    <t>jacobrlawrence24</t>
+  </si>
+  <si>
+    <t>calcifer_the_cavoodle</t>
+  </si>
+  <si>
+    <t>knowles2308sarah73</t>
+  </si>
+  <si>
+    <t>thewookaweens</t>
+  </si>
+  <si>
+    <t>maurice_meowington</t>
+  </si>
+  <si>
+    <t>labriverlife</t>
+  </si>
+  <si>
+    <t>maltese.yorkshire.luna</t>
+  </si>
+  <si>
+    <t>mavsmajesticmoments</t>
+  </si>
+  <si>
+    <t>heike_b_kish</t>
+  </si>
+  <si>
+    <t>adventures_wtih_alfie</t>
+  </si>
+  <si>
+    <t>cocotteduturfu</t>
+  </si>
+  <si>
+    <t>snoopywoodstock2024</t>
+  </si>
+  <si>
+    <t>world.of.pip</t>
+  </si>
+  <si>
+    <t>gift</t>
+  </si>
+  <si>
+    <t>sizuthebordercollie</t>
+  </si>
+  <si>
+    <t>littlemissbeverly_</t>
+  </si>
+  <si>
+    <t>queen_peanut23</t>
+  </si>
+  <si>
+    <t>barlowsgarden</t>
+  </si>
+  <si>
+    <t>littlekim94</t>
+  </si>
+  <si>
+    <t>sylphrena_lil_bit</t>
+  </si>
+  <si>
+    <t>chillin_withbenny</t>
+  </si>
+  <si>
+    <t>trixies.time</t>
+  </si>
+  <si>
+    <t>odinn_the_black_shephard</t>
+  </si>
+  <si>
+    <t>blueydawgg</t>
+  </si>
+  <si>
+    <t>bradytheblacklabpup</t>
+  </si>
+  <si>
+    <t>youngdumbarney</t>
+  </si>
+  <si>
+    <t>bianca_olmedo200</t>
+  </si>
+  <si>
+    <t>pixelgroot</t>
+  </si>
+  <si>
+    <t>callumjmckinlay</t>
+  </si>
+  <si>
+    <t>josephshanekusmierz</t>
+  </si>
+  <si>
+    <t>paalaal</t>
+  </si>
+  <si>
+    <t>denji_dooter</t>
+  </si>
+  <si>
+    <t>tourtel_27</t>
+  </si>
+  <si>
+    <t>makeupbytalaina</t>
+  </si>
+  <si>
+    <t>treyolberding</t>
+  </si>
+  <si>
+    <t>mbugglesworth</t>
+  </si>
+  <si>
+    <t>divinat0607</t>
+  </si>
+  <si>
+    <t>tandgadventures</t>
+  </si>
+  <si>
+    <t>bonnie_robens</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>bond_goldendoodle</t>
+  </si>
+  <si>
+    <t>henrythelabradude</t>
+  </si>
+  <si>
+    <t>lopezcasasbuenas</t>
+  </si>
+  <si>
+    <t>tobythegolden6</t>
+  </si>
+  <si>
+    <t>rue</t>
+  </si>
+  <si>
+    <t>castagna2013</t>
+  </si>
+  <si>
+    <t>nesstickles_</t>
+  </si>
+  <si>
+    <t>harlowthegoldenboy_</t>
+  </si>
+  <si>
+    <t>mary_michlovitch</t>
+  </si>
+  <si>
+    <t>maple_the_labpup</t>
+  </si>
+  <si>
+    <t>cookiethedoxie_24</t>
+  </si>
+  <si>
+    <t>chiquitathedach</t>
+  </si>
+  <si>
+    <t>buster.the.cane.corso_</t>
+  </si>
+  <si>
+    <t>hoosier_bassethound</t>
+  </si>
+  <si>
+    <t>jumbowoofs</t>
+  </si>
+  <si>
+    <t>guinness_doing_frenchie_things</t>
+  </si>
+  <si>
+    <t>priyah_capri_roise</t>
+  </si>
+  <si>
+    <t>lady_pippa_the_magnificent</t>
+  </si>
+  <si>
+    <t>mstajthepoddle</t>
+  </si>
+  <si>
+    <t>luna.m.m_capricorn</t>
+  </si>
+  <si>
+    <t>lily_bellejan2021</t>
+  </si>
+  <si>
+    <t>allthefurandfriends</t>
+  </si>
+  <si>
+    <t>htxteddy</t>
+  </si>
+  <si>
+    <t>mrmeekodoodle</t>
+  </si>
+  <si>
+    <t>a_beagle_named_chase</t>
+  </si>
+  <si>
+    <t>simba_schnuffi</t>
+  </si>
+  <si>
+    <t>the_henson_bunch</t>
+  </si>
+  <si>
+    <t>hele_9416</t>
+  </si>
+  <si>
+    <t>toni.schaferhund</t>
+  </si>
+  <si>
+    <t>turtlelatteva</t>
+  </si>
+  <si>
+    <t>cashthefriendlybully</t>
+  </si>
+  <si>
+    <t>connornbernie</t>
+  </si>
+  <si>
+    <t>kodathechow2024</t>
+  </si>
+  <si>
+    <t>fotomani_strom_annika</t>
+  </si>
+  <si>
+    <t>zeusandalfa</t>
+  </si>
+  <si>
+    <t>drei_samtpfoten3</t>
+  </si>
+  <si>
+    <t>corgikaitx</t>
+  </si>
+  <si>
+    <t>liloguzman23</t>
+  </si>
+  <si>
+    <t>mapleee_gworlll</t>
+  </si>
+  <si>
+    <t>archie_the_tabby</t>
+  </si>
+  <si>
+    <t>larrythegp_and_friends</t>
+  </si>
+  <si>
+    <t>squidgemont</t>
+  </si>
+  <si>
+    <t>itspudy_buddy</t>
+  </si>
+  <si>
+    <t>oreo.adventures.family</t>
+  </si>
+  <si>
+    <t>lunatheweenie661</t>
+  </si>
+  <si>
+    <t>onboutcash</t>
+  </si>
+  <si>
+    <t>cooperplaytime</t>
+  </si>
+  <si>
+    <t>yorkiesontheroad</t>
+  </si>
+  <si>
+    <t>thortheenglishcreamm</t>
+  </si>
+  <si>
+    <t>ebing2972</t>
+  </si>
+  <si>
+    <t>hawaiian_coco_</t>
+  </si>
+  <si>
+    <t>ogatobarth</t>
+  </si>
+  <si>
+    <t>grizabella_and_tinkerbell</t>
+  </si>
+  <si>
+    <t>newton_the_boykin</t>
+  </si>
+  <si>
+    <t>fijithepug_</t>
+  </si>
+  <si>
+    <t>ginger_corgi_ma_non_corgi</t>
+  </si>
+  <si>
+    <t>grandma_c_w</t>
+  </si>
+  <si>
+    <t>lolasaltthefrenchie</t>
+  </si>
+  <si>
+    <t>reginald_firstofhisname</t>
+  </si>
+  <si>
+    <t>debra_balloch</t>
+  </si>
+  <si>
+    <t>theoghosty</t>
+  </si>
+  <si>
+    <t>charliegarrigan</t>
+  </si>
+  <si>
+    <t>pibtheperrrfect</t>
+  </si>
+  <si>
+    <t>littlemissnalabean</t>
+  </si>
+  <si>
+    <t>odie_the_terrier_</t>
+  </si>
+  <si>
+    <t>rize_meow222</t>
+  </si>
+  <si>
+    <t>lunarnightmare629</t>
+  </si>
+  <si>
+    <t>pandatheamericanakita</t>
+  </si>
+  <si>
+    <t>athos_amstaffy</t>
   </si>
 </sst>
 </file>
@@ -63,7 +408,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +418,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -89,10 +446,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -408,38 +771,653 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5445F-36CD-4558-B0A4-BAF7727E9ABC}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>